<commit_message>
update small_strategic_case_study, update tests
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_Treatment_Demo.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_Treatment_Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1AFE0-CEDB-482F-B9AD-716C2E20363B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337D9A95-454F-465C-BC20-37E2C9F5E241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-5550" yWindow="-13455" windowWidth="17280" windowHeight="9885" tabRatio="834" firstSheet="41" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2248,121 +2248,48 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>84949</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>43851</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>141717</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="Group 4">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF046D9-B777-8894-5A9C-9B69EF8DA434}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACF0715-8C0C-5BA8-B3C4-D41F89DC3FAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="358140" y="238125"/>
-          <a:ext cx="12563475" cy="5639929"/>
-          <a:chOff x="0" y="102870"/>
-          <a:chExt cx="12563475" cy="5643739"/>
+          <a:off x="180975" y="400050"/>
+          <a:ext cx="13912251" cy="5351892"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Picture 1">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{217C791C-DB06-B32D-CBC7-34CCB4447D84}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="0" y="235565"/>
-            <a:ext cx="12308821" cy="5511044"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A47F8E1D-4567-818C-F857-53DAA9123266}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9946005" y="102870"/>
-            <a:ext cx="2617470" cy="750570"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5573,7 +5500,9 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA17" sqref="AA17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9584,9 +9513,7 @@
   </sheetPr>
   <dimension ref="A1:BD16"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView showZeros="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10301,9 +10228,7 @@
   </sheetPr>
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13626,9 +13551,7 @@
   </sheetPr>
   <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14202,9 +14125,7 @@
   </sheetPr>
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="S24" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView showZeros="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22545,9 +22466,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22623,9 +22542,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22684,9 +22601,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22832,9 +22747,7 @@
   </sheetPr>
   <dimension ref="A1:BA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23543,9 +23456,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23605,9 +23516,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23658,9 +23567,7 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23871,7 +23778,7 @@
   <dimension ref="A1:BD18"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -25100,9 +25007,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25178,9 +25083,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25484,9 +25387,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25545,9 +25446,7 @@
   </sheetPr>
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33871,9 +33770,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33924,9 +33821,7 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34113,9 +34008,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:F19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34503,9 +34396,7 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34671,9 +34562,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34740,9 +34629,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35061,9 +34948,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35130,8 +35015,8 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -35661,7 +35546,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
+      <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -35782,9 +35667,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35829,7 +35712,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:E6"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5:E6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42703,9 +42586,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -42846,9 +42727,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -42923,9 +42802,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43000,7 +42877,9 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43500,7 +43379,9 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -43649,9 +43530,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43819,9 +43698,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43879,9 +43756,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
initial changes to strategic model, treatment demo data, documentation, and tests
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_Treatment_Demo.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_Treatment_Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E52906-D1D1-4902-8845-3E93324CE570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1F9B5-0772-410C-B761-80F5E894D917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="12" activeTab="30" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2057,10 +2057,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2363,7 +2359,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8299,7 +8295,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -8341,9 +8337,7 @@
       <c r="A3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="10">
-        <v>1</v>
-      </c>
+      <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -8355,9 +8349,7 @@
         <v>137</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -8369,9 +8361,7 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="32"/>
@@ -8383,9 +8373,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
+      <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="32"/>
     </row>
@@ -8397,9 +8385,7 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
+      <c r="F7" s="10"/>
       <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8411,9 +8397,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="12">
-        <v>1</v>
-      </c>
+      <c r="G8" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>